<commit_message>
modified:   analysis_results/voltage_comparison_results.xlsx 	new file:   data/test_case2.xlsx 	new file:   data/test_case2_result.xlsx 	deleted:    "data/\347\237\263\346\241\245F12\350\215\211\346\262\263F27\344\272\244\347\233\264\346\265\201.xlsx" 	deleted:    "data/\347\237\263\346\241\245F12\350\215\211\346\262\263F27\344\272\244\347\233\264\346\265\201result.xlsx" 	modified:   test/test_runhpf.jl 	modified:   test/test_runhpf_gpu.jl 	new file:   topology_results.xlsx 	new file:   topology_results_partition_report.xlsx
</commit_message>
<xml_diff>
--- a/analysis_results/voltage_comparison_results.xlsx
+++ b/analysis_results/voltage_comparison_results.xlsx
@@ -49,13 +49,13 @@
     <t>Mag_Within_Tolerance</t>
   </si>
   <si>
-    <t>Bus_大刀沙村2号直流</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙村3号直流</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙村5号直流</t>
+    <t>dcBus_3</t>
+  </si>
+  <si>
+    <t>dcBus_2</t>
+  </si>
+  <si>
+    <t>dcBus_1</t>
   </si>
   <si>
     <t>Calc_Volt_Ang</t>
@@ -70,214 +70,214 @@
     <t>Ang_Within_Tolerance</t>
   </si>
   <si>
-    <t>Bus_01塔</t>
-  </si>
-  <si>
-    <t>Bus_02塔</t>
-  </si>
-  <si>
-    <t>Bus_03杆</t>
-  </si>
-  <si>
-    <t>Bus_06杆</t>
-  </si>
-  <si>
-    <t>Bus_08塔</t>
-  </si>
-  <si>
-    <t>Bus_10塔</t>
-  </si>
-  <si>
-    <t>Bus_11杆</t>
-  </si>
-  <si>
-    <t>Bus_13塔</t>
-  </si>
-  <si>
-    <t>Bus_21杆</t>
-  </si>
-  <si>
-    <t>Bus_26塔</t>
-  </si>
-  <si>
-    <t>Bus_28塔</t>
-  </si>
-  <si>
-    <t>Bus_28杆</t>
-  </si>
-  <si>
-    <t>Bus_30杆</t>
-  </si>
-  <si>
-    <t>Bus_35杆</t>
-  </si>
-  <si>
-    <t>Bus_52杆</t>
-  </si>
-  <si>
-    <t>Bus_76杆</t>
-  </si>
-  <si>
-    <t>Bus_京毅开关房</t>
-  </si>
-  <si>
-    <t>Bus_信强贸易开关</t>
-  </si>
-  <si>
-    <t>Bus_八糖尾鱼塘支01杆</t>
-  </si>
-  <si>
-    <t>Bus_八糖鱼45杆</t>
-  </si>
-  <si>
-    <t>Bus_南派1号电缆分接箱</t>
-  </si>
-  <si>
-    <t>Bus_南清干01杆</t>
-  </si>
-  <si>
-    <t>Bus_南清干04塔开关</t>
-  </si>
-  <si>
-    <t>Bus_南清干14杆开关</t>
-  </si>
-  <si>
-    <t>Bus_南清干24杆开关</t>
-  </si>
-  <si>
-    <t>Bus_南清干27塔开关</t>
-  </si>
-  <si>
-    <t>Bus_南清干45塔与清流干01</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙支01杆</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙支18杆</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙支28+1杆</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙支30杆</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙支42杆</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙支53杆</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙支64杆</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙支77塔</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙村1号</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙村2号</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙村3号</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙村4号</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙村5号</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙村合作经济社</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙水厂_中压</t>
-  </si>
-  <si>
-    <t>Bus_大刀沙水厂_交流</t>
-  </si>
-  <si>
-    <t>Bus_市南路1号电缆分接箱</t>
-  </si>
-  <si>
-    <t>Bus_桥发支01杆</t>
-  </si>
-  <si>
-    <t>Bus_桥发支19塔开关</t>
-  </si>
-  <si>
-    <t>Bus_沙龙干01杆</t>
-  </si>
-  <si>
-    <t>Bus_沙龙干03塔开关</t>
-  </si>
-  <si>
-    <t>Bus_沙龙干20杆开关</t>
-  </si>
-  <si>
-    <t>Bus_沙龙干33塔开关</t>
-  </si>
-  <si>
-    <t>Bus_沙龙干44塔开关</t>
-  </si>
-  <si>
-    <t>Bus_清河东路电缆分接箱</t>
-  </si>
-  <si>
-    <t>Bus_清流1号支16杆</t>
-  </si>
-  <si>
-    <t>Bus_清流1号电缆分接箱</t>
-  </si>
-  <si>
-    <t>Bus_清流干08塔</t>
-  </si>
-  <si>
-    <t>Bus_清流干19杆开关</t>
-  </si>
-  <si>
-    <t>Bus_清流村会堂2号高低压开关</t>
-  </si>
-  <si>
-    <t>Bus_清流村经济合作社开关房</t>
-  </si>
-  <si>
-    <t>Bus_清流观龙18队</t>
-  </si>
-  <si>
-    <t>Bus_石楼F12</t>
-  </si>
-  <si>
-    <t>Bus_石楼F22</t>
-  </si>
-  <si>
-    <t>Bus_草河F7</t>
-  </si>
-  <si>
-    <t>Bus_草河F27</t>
-  </si>
-  <si>
-    <t>Bus_草河村22号高低开关房</t>
-  </si>
-  <si>
-    <t>Bus_草河村32号欧式箱变</t>
-  </si>
-  <si>
-    <t>Bus_裕丰13塔</t>
-  </si>
-  <si>
-    <t>Bus_裕丰F19</t>
-  </si>
-  <si>
-    <t>Bus_观龙大站2号高低压开关房</t>
-  </si>
-  <si>
-    <t>Bus_观龙大站支01杆</t>
-  </si>
-  <si>
-    <t>Bus_观龙大站高低压开关房</t>
+    <t>Bus_33</t>
+  </si>
+  <si>
+    <t>Bus_56</t>
+  </si>
+  <si>
+    <t>Bus_38</t>
+  </si>
+  <si>
+    <t>Bus_37</t>
+  </si>
+  <si>
+    <t>Bus_54</t>
+  </si>
+  <si>
+    <t>Bus_17</t>
+  </si>
+  <si>
+    <t>Bus_18</t>
+  </si>
+  <si>
+    <t>Bus_6</t>
+  </si>
+  <si>
+    <t>Bus_42</t>
+  </si>
+  <si>
+    <t>Bus_48</t>
+  </si>
+  <si>
+    <t>Bus_67</t>
+  </si>
+  <si>
+    <t>Bus_46</t>
+  </si>
+  <si>
+    <t>Bus_41</t>
+  </si>
+  <si>
+    <t>Bus_13</t>
+  </si>
+  <si>
+    <t>Bus_40</t>
+  </si>
+  <si>
+    <t>Bus_31</t>
+  </si>
+  <si>
+    <t>Bus_62</t>
+  </si>
+  <si>
+    <t>Bus_63</t>
+  </si>
+  <si>
+    <t>Bus_66</t>
+  </si>
+  <si>
+    <t>Bus_68</t>
+  </si>
+  <si>
+    <t>Bus_58</t>
+  </si>
+  <si>
+    <t>Bus_57</t>
+  </si>
+  <si>
+    <t>Bus_55</t>
+  </si>
+  <si>
+    <t>Bus_52</t>
+  </si>
+  <si>
+    <t>Bus_51</t>
+  </si>
+  <si>
+    <t>Bus_47</t>
+  </si>
+  <si>
+    <t>Bus_45</t>
+  </si>
+  <si>
+    <t>Bus_15</t>
+  </si>
+  <si>
+    <t>Bus_19</t>
+  </si>
+  <si>
+    <t>Bus_24</t>
+  </si>
+  <si>
+    <t>Bus_23</t>
+  </si>
+  <si>
+    <t>Bus_25</t>
+  </si>
+  <si>
+    <t>Bus_27</t>
+  </si>
+  <si>
+    <t>Bus_29</t>
+  </si>
+  <si>
+    <t>Bus_32</t>
+  </si>
+  <si>
+    <t>Bus_28</t>
+  </si>
+  <si>
+    <t>Bus_22</t>
+  </si>
+  <si>
+    <t>Bus_21</t>
+  </si>
+  <si>
+    <t>Bus_30</t>
+  </si>
+  <si>
+    <t>Bus_20</t>
+  </si>
+  <si>
+    <t>Bus_26</t>
+  </si>
+  <si>
+    <t>Bus_16</t>
+  </si>
+  <si>
+    <t>Bus_70</t>
+  </si>
+  <si>
+    <t>Bus_2</t>
+  </si>
+  <si>
+    <t>Bus_9</t>
+  </si>
+  <si>
+    <t>Bus_10</t>
+  </si>
+  <si>
+    <t>Bus_4</t>
+  </si>
+  <si>
+    <t>Bus_5</t>
+  </si>
+  <si>
+    <t>Bus_11</t>
+  </si>
+  <si>
+    <t>Bus_12</t>
+  </si>
+  <si>
+    <t>Bus_14</t>
+  </si>
+  <si>
+    <t>Bus_59</t>
+  </si>
+  <si>
+    <t>Bus_50</t>
+  </si>
+  <si>
+    <t>Bus_49</t>
+  </si>
+  <si>
+    <t>Bus_44</t>
+  </si>
+  <si>
+    <t>Bus_43</t>
+  </si>
+  <si>
+    <t>Bus_69</t>
+  </si>
+  <si>
+    <t>Bus_64</t>
+  </si>
+  <si>
+    <t>Bus_39</t>
+  </si>
+  <si>
+    <t>Bus_60</t>
+  </si>
+  <si>
+    <t>Bus_65</t>
+  </si>
+  <si>
+    <t>Bus_8</t>
+  </si>
+  <si>
+    <t>Bus_1</t>
+  </si>
+  <si>
+    <t>Bus_3</t>
+  </si>
+  <si>
+    <t>Bus_7</t>
+  </si>
+  <si>
+    <t>Bus_53</t>
+  </si>
+  <si>
+    <t>Bus_61</t>
+  </si>
+  <si>
+    <t>Bus_35</t>
+  </si>
+  <si>
+    <t>Bus_36</t>
+  </si>
+  <si>
+    <t>Bus_34</t>
   </si>
 </sst>
 </file>

</xml_diff>